<commit_message>
fixed export issues and comparison result analysis
</commit_message>
<xml_diff>
--- a/sample_data/example_run1.xlsx
+++ b/sample_data/example_run1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic_Weizmann\WIS_pythonGabor\Coding\ODyssey\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777A99E2-DFF5-4F1E-9C0C-AC87A1FF9D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359D6D4E-7677-4913-A275-73A774B682CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{83AB0913-2B68-40BB-A5C7-B40C6383A6EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{83AB0913-2B68-40BB-A5C7-B40C6383A6EA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Time_min</t>
   </si>
@@ -65,15 +66,39 @@
   <si>
     <t>TreatmentC_rep2</t>
   </si>
+  <si>
+    <t>Time_hours</t>
+  </si>
+  <si>
+    <t>time (mins)</t>
+  </si>
+  <si>
+    <t>TreatmentA_rep3</t>
+  </si>
+  <si>
+    <t>TreatmentB_rep3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,8 +124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +463,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762BDB2-0983-4299-AE04-950488AF693D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5DA0F4-F1B7-4AD6-ABA7-8C5DDEE8EA55}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -477,28 +506,28 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.2999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C2">
-        <v>4.9000000000000002E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D2">
-        <v>3.9E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E2">
-        <v>2.9000000000000001E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="F2">
-        <v>0.06</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="G2">
-        <v>-4.0000000000000001E-3</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="H2">
-        <v>0.09</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="I2">
-        <v>0.04</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -506,28 +535,28 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>5.0999999999999997E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C3">
-        <v>0.05</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D3">
-        <v>9.1999999999999998E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E3">
-        <v>2.1000000000000001E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F3">
-        <v>4.7E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G3">
-        <v>4.4999999999999998E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H3">
-        <v>9.0999999999999998E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="I3">
-        <v>4.7E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -535,28 +564,28 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C4">
-        <v>4.8000000000000001E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="D4">
-        <v>7.5999999999999998E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E4">
-        <v>8.6999999999999994E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F4">
-        <v>4.2000000000000003E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="G4">
-        <v>8.6999999999999994E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="H4">
-        <v>0.10100000000000001</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="I4">
-        <v>9.2999999999999999E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -564,28 +593,28 @@
         <v>30</v>
       </c>
       <c r="B5">
-        <v>5.1999999999999998E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C5">
-        <v>4.9000000000000002E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D5">
-        <v>8.5000000000000006E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E5">
-        <v>6.9000000000000006E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="F5">
-        <v>6.9000000000000006E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="G5">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="H5">
-        <v>8.2000000000000003E-2</v>
+        <v>0.13</v>
       </c>
       <c r="I5">
-        <v>8.7999999999999995E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -593,28 +622,28 @@
         <v>40</v>
       </c>
       <c r="B6">
-        <v>4.9000000000000002E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C6">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="D6">
-        <v>8.6999999999999994E-2</v>
+        <v>0.114</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F6">
-        <v>6.3E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="G6">
-        <v>0.09</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="H6">
-        <v>0.14299999999999999</v>
+        <v>0.114</v>
       </c>
       <c r="I6">
-        <v>0.125</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -622,28 +651,28 @@
         <v>50</v>
       </c>
       <c r="B7">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="C7">
-        <v>4.8000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D7">
-        <v>8.5000000000000006E-2</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="E7">
-        <v>0.13400000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="F7">
-        <v>8.5999999999999993E-2</v>
+        <v>0.104</v>
       </c>
       <c r="G7">
-        <v>7.1999999999999995E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="H7">
-        <v>0.114</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="I7">
-        <v>0.152</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -651,28 +680,28 @@
         <v>60</v>
       </c>
       <c r="B8">
-        <v>0.05</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C8">
-        <v>5.0999999999999997E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D8">
-        <v>0.20599999999999999</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="E8">
-        <v>0.193</v>
+        <v>0.184</v>
       </c>
       <c r="F8">
-        <v>0.14699999999999999</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="G8">
-        <v>0.16300000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="H8">
-        <v>0.216</v>
+        <v>0.214</v>
       </c>
       <c r="I8">
-        <v>0.23200000000000001</v>
+        <v>0.21199999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -680,28 +709,28 @@
         <v>70</v>
       </c>
       <c r="B9">
-        <v>5.1999999999999998E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C9">
-        <v>5.1999999999999998E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D9">
-        <v>0.30599999999999999</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="E9">
-        <v>0.318</v>
+        <v>0.307</v>
       </c>
       <c r="F9">
+        <v>0.247</v>
+      </c>
+      <c r="G9">
         <v>0.24</v>
       </c>
-      <c r="G9">
-        <v>0.28000000000000003</v>
-      </c>
       <c r="H9">
-        <v>0.34</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="I9">
-        <v>0.32400000000000001</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -709,28 +738,28 @@
         <v>80</v>
       </c>
       <c r="B10">
-        <v>5.0999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="C10">
-        <v>0.05</v>
+        <v>4.7E-2</v>
       </c>
       <c r="D10">
-        <v>0.42299999999999999</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="E10">
-        <v>0.43</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="F10">
-        <v>0.38400000000000001</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="G10">
-        <v>0.312</v>
+        <v>0.317</v>
       </c>
       <c r="H10">
-        <v>0.41099999999999998</v>
+        <v>0.436</v>
       </c>
       <c r="I10">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -738,28 +767,28 @@
         <v>90</v>
       </c>
       <c r="B11">
-        <v>0.05</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C11">
-        <v>5.1999999999999998E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="D11">
-        <v>0.50600000000000001</v>
+        <v>0.497</v>
       </c>
       <c r="E11">
-        <v>0.46</v>
+        <v>0.52100000000000002</v>
       </c>
       <c r="F11">
-        <v>0.41899999999999998</v>
+        <v>0.42099999999999999</v>
       </c>
       <c r="G11">
-        <v>0.442</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="H11">
-        <v>0.55500000000000005</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="I11">
-        <v>0.56499999999999995</v>
+        <v>0.55700000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -767,28 +796,28 @@
         <v>100</v>
       </c>
       <c r="B12">
-        <v>0.05</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C12">
         <v>0.05</v>
       </c>
       <c r="D12">
-        <v>0.60399999999999998</v>
+        <v>0.628</v>
       </c>
       <c r="E12">
-        <v>0.60799999999999998</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="F12">
-        <v>0.51400000000000001</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="G12">
-        <v>0.51200000000000001</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="H12">
-        <v>0.64700000000000002</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="I12">
-        <v>0.66800000000000004</v>
+        <v>0.66200000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -796,28 +825,28 @@
         <v>110</v>
       </c>
       <c r="B13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C13">
         <v>0.05</v>
       </c>
-      <c r="C13">
-        <v>5.1999999999999998E-2</v>
-      </c>
       <c r="D13">
-        <v>0.72399999999999998</v>
+        <v>0.69099999999999995</v>
       </c>
       <c r="E13">
-        <v>0.70399999999999996</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="F13">
-        <v>0.58699999999999997</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="G13">
-        <v>0.58199999999999996</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="H13">
-        <v>0.77800000000000002</v>
+        <v>0.77300000000000002</v>
       </c>
       <c r="I13">
-        <v>0.77200000000000002</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -825,28 +854,28 @@
         <v>120</v>
       </c>
       <c r="B14">
-        <v>4.9000000000000002E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C14">
         <v>0.05</v>
       </c>
       <c r="D14">
-        <v>0.78800000000000003</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="E14">
-        <v>0.81399999999999995</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="F14">
-        <v>0.67100000000000004</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="G14">
-        <v>0.70399999999999996</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="H14">
-        <v>0.88800000000000001</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="I14">
-        <v>0.89200000000000002</v>
+        <v>0.879</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -854,28 +883,28 @@
         <v>130</v>
       </c>
       <c r="B15">
-        <v>4.8000000000000001E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C15">
         <v>0.05</v>
       </c>
       <c r="D15">
-        <v>0.91500000000000004</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="E15">
-        <v>0.88100000000000001</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="F15">
-        <v>0.76</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="G15">
-        <v>0.76600000000000001</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="H15">
-        <v>0.96299999999999997</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="I15">
-        <v>0.996</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -883,28 +912,28 @@
         <v>140</v>
       </c>
       <c r="B16">
-        <v>5.1999999999999998E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C16">
-        <v>4.8000000000000001E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D16">
-        <v>1.0069999999999999</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="E16">
-        <v>0.97399999999999998</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="F16">
-        <v>0.84899999999999998</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="G16">
-        <v>0.81799999999999995</v>
+        <v>0.87</v>
       </c>
       <c r="H16">
-        <v>1.1220000000000001</v>
+        <v>1.091</v>
       </c>
       <c r="I16">
-        <v>1.1080000000000001</v>
+        <v>1.1279999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -912,28 +941,28 @@
         <v>150</v>
       </c>
       <c r="B17">
-        <v>0.05</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C17">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="D17">
-        <v>1.0249999999999999</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="E17">
-        <v>1.0389999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="F17">
-        <v>0.81299999999999994</v>
+        <v>0.82099999999999995</v>
       </c>
       <c r="G17">
-        <v>0.875</v>
+        <v>0.84</v>
       </c>
       <c r="H17">
-        <v>1.133</v>
+        <v>1.107</v>
       </c>
       <c r="I17">
-        <v>1.107</v>
+        <v>1.099</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -941,28 +970,28 @@
         <v>160</v>
       </c>
       <c r="B18">
-        <v>4.8000000000000001E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="C18">
-        <v>5.1999999999999998E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D18">
-        <v>1.0089999999999999</v>
+        <v>1.0189999999999999</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>1.0329999999999999</v>
       </c>
       <c r="F18">
-        <v>0.83599999999999997</v>
+        <v>0.876</v>
       </c>
       <c r="G18">
-        <v>0.872</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="H18">
-        <v>1.1299999999999999</v>
+        <v>1.075</v>
       </c>
       <c r="I18">
-        <v>1.101</v>
+        <v>1.095</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -970,7 +999,7 @@
         <v>170</v>
       </c>
       <c r="B19">
-        <v>5.0999999999999997E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C19">
         <v>4.8000000000000001E-2</v>
@@ -979,19 +1008,19 @@
         <v>1.0409999999999999</v>
       </c>
       <c r="E19">
-        <v>1.026</v>
+        <v>1.0129999999999999</v>
       </c>
       <c r="F19">
-        <v>0.86799999999999999</v>
+        <v>0.879</v>
       </c>
       <c r="G19">
-        <v>0.86899999999999999</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="H19">
-        <v>1.145</v>
+        <v>1.151</v>
       </c>
       <c r="I19">
-        <v>1.143</v>
+        <v>1.127</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -999,28 +1028,28 @@
         <v>180</v>
       </c>
       <c r="B20">
-        <v>5.0999999999999997E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C20">
         <v>0.05</v>
       </c>
       <c r="D20">
-        <v>1.0389999999999999</v>
+        <v>1.0529999999999999</v>
       </c>
       <c r="E20">
-        <v>1.05</v>
+        <v>1.0349999999999999</v>
       </c>
       <c r="F20">
-        <v>0.88700000000000001</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="G20">
-        <v>0.89600000000000002</v>
+        <v>0.85199999999999998</v>
       </c>
       <c r="H20">
-        <v>1.135</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I20">
-        <v>1.093</v>
+        <v>1.1559999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1028,28 +1057,28 @@
         <v>190</v>
       </c>
       <c r="B21">
-        <v>5.1999999999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C21">
-        <v>5.3999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D21">
-        <v>1.0589999999999999</v>
+        <v>1.046</v>
       </c>
       <c r="E21">
-        <v>1.048</v>
+        <v>1.06</v>
       </c>
       <c r="F21">
-        <v>0.89</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="G21">
-        <v>0.89</v>
+        <v>0.90300000000000002</v>
       </c>
       <c r="H21">
-        <v>1.155</v>
+        <v>1.137</v>
       </c>
       <c r="I21">
-        <v>1.133</v>
+        <v>1.147</v>
       </c>
     </row>
   </sheetData>
@@ -1058,18 +1087,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5DA0F4-F1B7-4AD6-ABA7-8C5DDEE8EA55}">
-  <dimension ref="A1:I21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762BDB2-0983-4299-AE04-950488AF693D}">
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1101,294 +1130,294 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.0999999999999997E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C2">
-        <v>4.8000000000000001E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="D2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="E2">
-        <v>6.3E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="F2">
-        <v>7.1999999999999995E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="G2">
-        <v>5.3999999999999999E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="H2">
-        <v>7.9000000000000001E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="I2">
-        <v>8.8999999999999996E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>10</v>
+        <v>0.25</v>
       </c>
       <c r="B3">
-        <v>5.1999999999999998E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C3">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="D3">
-        <v>0.06</v>
+        <v>6.3E-2</v>
       </c>
       <c r="E3">
-        <v>7.4999999999999997E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="F3">
-        <v>4.4999999999999998E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="G3">
-        <v>6.2E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H3">
-        <v>3.6999999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="I3">
-        <v>5.1999999999999998E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>20</v>
+        <v>0.5</v>
       </c>
       <c r="B4">
-        <v>5.0999999999999997E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C4">
-        <v>4.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D4">
-        <v>5.2999999999999999E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="E4">
-        <v>7.4999999999999997E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="F4">
-        <v>2.9000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G4">
-        <v>6.5000000000000002E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="H4">
-        <v>6.7000000000000004E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="I4">
-        <v>7.6999999999999999E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>30</v>
+        <v>0.75</v>
       </c>
       <c r="B5">
-        <v>4.9000000000000002E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C5">
         <v>0.05</v>
       </c>
       <c r="D5">
-        <v>7.5999999999999998E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="E5">
-        <v>8.8999999999999996E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F5">
-        <v>6.2E-2</v>
+        <v>0.107</v>
       </c>
       <c r="G5">
-        <v>8.5000000000000006E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="H5">
-        <v>0.13</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I5">
-        <v>0.1</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>0.05</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D6">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E6">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F6">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="D6">
-        <v>0.114</v>
-      </c>
-      <c r="E6">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="F6">
-        <v>6.9000000000000006E-2</v>
-      </c>
       <c r="G6">
-        <v>9.6000000000000002E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H6">
-        <v>0.114</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="I6">
-        <v>0.13200000000000001</v>
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>50</v>
+        <v>1.25</v>
       </c>
       <c r="B7">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C7">
-        <v>4.9000000000000002E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D7">
-        <v>0.10299999999999999</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="E7">
-        <v>0.13500000000000001</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="F7">
-        <v>0.104</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="G7">
-        <v>9.9000000000000005E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="H7">
-        <v>0.13600000000000001</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="I7">
-        <v>9.8000000000000004E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>60</v>
+        <v>1.5</v>
       </c>
       <c r="B8">
-        <v>5.0999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="C8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.08</v>
+      </c>
+      <c r="F8">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G8">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D8">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="E8">
-        <v>0.184</v>
-      </c>
-      <c r="F8">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="G8">
-        <v>0.17799999999999999</v>
-      </c>
       <c r="H8">
-        <v>0.214</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="I8">
-        <v>0.21199999999999999</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>70</v>
+        <v>1.75</v>
       </c>
       <c r="B9">
-        <v>5.0999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C9">
-        <v>4.9000000000000002E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D9">
-        <v>0.26400000000000001</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="E9">
-        <v>0.307</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="F9">
-        <v>0.247</v>
+        <v>0.104</v>
       </c>
       <c r="G9">
-        <v>0.24</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="H9">
-        <v>0.29899999999999999</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="I9">
-        <v>0.35</v>
+        <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>4.5999999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C10">
-        <v>4.7E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D10">
-        <v>0.39400000000000002</v>
+        <v>0.19</v>
       </c>
       <c r="E10">
-        <v>0.42499999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="F10">
-        <v>0.36599999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="G10">
-        <v>0.317</v>
+        <v>0.189</v>
       </c>
       <c r="H10">
-        <v>0.436</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="I10">
-        <v>0.41</v>
+        <v>0.20699999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>90</v>
+        <v>2.25</v>
       </c>
       <c r="B11">
-        <v>5.1999999999999998E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C11">
-        <v>4.7E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D11">
-        <v>0.497</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="E11">
-        <v>0.52100000000000002</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="F11">
-        <v>0.42099999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="G11">
-        <v>0.45400000000000001</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="H11">
-        <v>0.53300000000000003</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="I11">
-        <v>0.55700000000000005</v>
+        <v>0.34100000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>100</v>
+        <v>2.5</v>
       </c>
       <c r="B12">
         <v>5.1999999999999998E-2</v>
@@ -1397,286 +1426,2664 @@
         <v>0.05</v>
       </c>
       <c r="D12">
-        <v>0.628</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="E12">
-        <v>0.61099999999999999</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="F12">
-        <v>0.47699999999999998</v>
+        <v>0.34699999999999998</v>
       </c>
       <c r="G12">
-        <v>0.58899999999999997</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="H12">
-        <v>0.67300000000000004</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="I12">
-        <v>0.66200000000000003</v>
+        <v>0.495</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>110</v>
+        <v>2.75</v>
       </c>
       <c r="B13">
-        <v>4.7E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C13">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D13">
-        <v>0.69099999999999995</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="E13">
-        <v>0.71299999999999997</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="F13">
-        <v>0.60199999999999998</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="G13">
-        <v>0.63200000000000001</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="H13">
-        <v>0.77300000000000002</v>
+        <v>0.61</v>
       </c>
       <c r="I13">
-        <v>0.78</v>
+        <v>0.60099999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="B14">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C14">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="C14">
-        <v>0.05</v>
-      </c>
       <c r="D14">
-        <v>0.79600000000000004</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="E14">
-        <v>0.82199999999999995</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="F14">
-        <v>0.69599999999999995</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="G14">
-        <v>0.66700000000000004</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="H14">
-        <v>0.85799999999999998</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="I14">
-        <v>0.879</v>
+        <v>0.68899999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>130</v>
+        <v>3.25</v>
       </c>
       <c r="B15">
-        <v>5.1999999999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C15">
-        <v>0.05</v>
+        <v>5.5E-2</v>
       </c>
       <c r="D15">
-        <v>0.93500000000000005</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="E15">
-        <v>0.88400000000000001</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="F15">
-        <v>0.76800000000000002</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="G15">
-        <v>0.71499999999999997</v>
+        <v>0.59</v>
       </c>
       <c r="H15">
-        <v>0.97799999999999998</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="I15">
-        <v>0.98399999999999999</v>
+        <v>0.75600000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>140</v>
+        <v>3.5</v>
       </c>
       <c r="B16">
-        <v>5.0999999999999997E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C16">
-        <v>5.2999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D16">
-        <v>1.0009999999999999</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="E16">
-        <v>1.0289999999999999</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="F16">
-        <v>0.86299999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G16">
-        <v>0.87</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="H16">
-        <v>1.091</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="I16">
-        <v>1.1279999999999999</v>
+        <v>0.72299999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>150</v>
+        <v>3.75</v>
       </c>
       <c r="B17">
-        <v>4.8000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C17">
-        <v>5.0999999999999997E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D17">
-        <v>0.98099999999999998</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="E17">
-        <v>0.99</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="F17">
-        <v>0.82099999999999995</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="G17">
-        <v>0.84</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="H17">
-        <v>1.107</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="I17">
-        <v>1.099</v>
+        <v>0.755</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>160</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>4.7E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C18">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="D18">
-        <v>1.0189999999999999</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="E18">
-        <v>1.0329999999999999</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="F18">
-        <v>0.876</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G18">
-        <v>0.84699999999999998</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="H18">
-        <v>1.075</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="I18">
-        <v>1.095</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>170</v>
-      </c>
-      <c r="B19">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="C19">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="D19">
-        <v>1.0409999999999999</v>
-      </c>
-      <c r="E19">
-        <v>1.0129999999999999</v>
-      </c>
-      <c r="F19">
-        <v>0.879</v>
-      </c>
-      <c r="G19">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="H19">
-        <v>1.151</v>
-      </c>
-      <c r="I19">
-        <v>1.127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>180</v>
-      </c>
-      <c r="B20">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="C20">
-        <v>0.05</v>
-      </c>
-      <c r="D20">
-        <v>1.0529999999999999</v>
-      </c>
-      <c r="E20">
-        <v>1.0349999999999999</v>
-      </c>
-      <c r="F20">
-        <v>0.89700000000000002</v>
-      </c>
-      <c r="G20">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="H20">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="I20">
-        <v>1.1559999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>190</v>
-      </c>
-      <c r="B21">
-        <v>0.05</v>
-      </c>
-      <c r="C21">
-        <v>0.05</v>
-      </c>
-      <c r="D21">
-        <v>1.046</v>
-      </c>
-      <c r="E21">
-        <v>1.06</v>
-      </c>
-      <c r="F21">
-        <v>0.88100000000000001</v>
-      </c>
-      <c r="G21">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="H21">
-        <v>1.137</v>
-      </c>
-      <c r="I21">
-        <v>1.147</v>
+        <v>0.73099999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21E111E-C884-4CBA-9297-D73AF9F94698}">
+  <dimension ref="A1:G182"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>19.333333333333332</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>29.333333333333329</v>
+      </c>
+      <c r="B4" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>39.333333333333336</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>49.333333333333329</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>59.333333333333336</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>69.333333333333329</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>79.333333333333329</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>89.333333333333343</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>99.333333333333329</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>109.33333333333334</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>119.33333333333334</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>129.33333333333331</v>
+      </c>
+      <c r="B14" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>139.33333333333331</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="C15" s="2">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>149.33333333333334</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.127</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>159.33333333333331</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.217</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>169.33333333333334</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.218</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.214</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>179.33333333333334</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.252</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.315</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.33800000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>189.33333333333331</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.314</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.318</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.316</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.372</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>199.33333333333331</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.379</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.371</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.373</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>209.33333333333334</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>219.33333333333334</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>229.33333333333334</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.61599999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>239.33333333333334</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.624</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>249.33333333333334</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>259.33333333333331</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.77700000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>269.33333333333331</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.749</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.749</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>279.33333333333337</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>289.33333333333331</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.876</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>299.33333333333331</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.871</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.90200000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>309.33333333333337</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.92600000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>319.33333333333331</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.94899999999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>329.33333333333331</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>339.33333333333337</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>349.33333333333331</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1.016</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>359.33333333333331</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1.002</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1.012</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.997</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1.038</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>369.33333333333331</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1.024</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1.012</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1.032</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1.016</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1.0369999999999999</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1.0569999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>379.33333333333326</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1.044</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1.0740000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>389.33333333333331</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1.075</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1.0680000000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1.069</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1.093</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>399.33333333333343</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1.083</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1.095</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1.0880000000000001</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1.109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>409.33333333333337</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1.083</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1.109</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="G42" s="2">
+        <v>1.1259999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>419.33333333333331</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1.099</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1.131</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1.119</v>
+      </c>
+      <c r="G43" s="2">
+        <v>1.1419999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>429.33333333333337</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1.137</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1.1160000000000001</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1.149</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1.135</v>
+      </c>
+      <c r="G44" s="2">
+        <v>1.1579999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>439.33333333333331</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1.153</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1.129</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1.149</v>
+      </c>
+      <c r="G45" s="2">
+        <v>1.1739999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>449.33333333333331</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1.143</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1.1779999999999999</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1.173</v>
+      </c>
+      <c r="F46" s="2">
+        <v>1.163</v>
+      </c>
+      <c r="G46" s="2">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>459.33333333333331</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1.1819999999999999</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1.1910000000000001</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1.1870000000000001</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1.177</v>
+      </c>
+      <c r="G47" s="2">
+        <v>1.204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>469.33333333333326</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1.196</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1.171</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="G48" s="2">
+        <v>1.2190000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>479.33333333333331</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1.2090000000000001</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1.1839999999999999</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="F49" s="2">
+        <v>1.202</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1.234</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>489.33333333333331</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1.2230000000000001</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1.1990000000000001</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1.2310000000000001</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1.212</v>
+      </c>
+      <c r="G50" s="2">
+        <v>1.2509999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>499.33333333333337</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1.236</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1.212</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1.242</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1.242</v>
+      </c>
+      <c r="F51" s="2">
+        <v>1.2230000000000001</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1.2609999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>509.33333333333331</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1.2230000000000001</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1.254</v>
+      </c>
+      <c r="E52" s="2">
+        <v>1.254</v>
+      </c>
+      <c r="F52" s="2">
+        <v>1.234</v>
+      </c>
+      <c r="G52" s="2">
+        <v>1.272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>519.33333333333326</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1.264</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1.2350000000000001</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1.2649999999999999</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1.2649999999999999</v>
+      </c>
+      <c r="F53" s="2">
+        <v>1.2450000000000001</v>
+      </c>
+      <c r="G53" s="2">
+        <v>1.2889999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>529.33333333333337</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1.276</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1.2450000000000001</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1.254</v>
+      </c>
+      <c r="G54" s="2">
+        <v>1.294</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>539.33333333333337</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1.288</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1.254</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1.284</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1.264</v>
+      </c>
+      <c r="G55" s="2">
+        <v>1.304</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>549.33333333333326</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1.2989999999999999</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1.262</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1.274</v>
+      </c>
+      <c r="G56" s="2">
+        <v>1.3149999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>559.33333333333337</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1.31</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1.2709999999999999</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1.3029999999999999</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1.3009999999999999</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1.2829999999999999</v>
+      </c>
+      <c r="G57" s="2">
+        <v>1.3220000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>569.33333333333337</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1.3220000000000001</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1.2789999999999999</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1.3089999999999999</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1.292</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1.331</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>579.33333333333326</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1.288</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1.321</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1.3169999999999999</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1.3009999999999999</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>589.33333333333337</v>
+      </c>
+      <c r="B60" s="2">
+        <v>1.3440000000000001</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1.296</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1.329</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1.3260000000000001</v>
+      </c>
+      <c r="F60" s="2">
+        <v>1.3089999999999999</v>
+      </c>
+      <c r="G60" s="2">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>599.33333333333337</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1.3540000000000001</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1.3029999999999999</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1.337</v>
+      </c>
+      <c r="E61" s="2">
+        <v>1.333</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1.3180000000000001</v>
+      </c>
+      <c r="G61" s="2">
+        <v>1.359</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>609.33333333333326</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1.363</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1.345</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1.341</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1.327</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1.369</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>619.33333333333337</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1.3720000000000001</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1.319</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1.353</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1.3480000000000001</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1.337</v>
+      </c>
+      <c r="G63" s="2">
+        <v>1.3779999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>629.33333333333337</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1.381</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1.3280000000000001</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1.363</v>
+      </c>
+      <c r="E64" s="2">
+        <v>1.355</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1.345</v>
+      </c>
+      <c r="G64" s="2">
+        <v>1.3879999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>639.33333333333326</v>
+      </c>
+      <c r="B65" s="2">
+        <v>1.39</v>
+      </c>
+      <c r="C65" s="2">
+        <v>1.335</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1.371</v>
+      </c>
+      <c r="E65" s="2">
+        <v>1.363</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1.3540000000000001</v>
+      </c>
+      <c r="G65" s="2">
+        <v>1.3959999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>649.33333333333337</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1.3979999999999999</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1.34</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1.3779999999999999</v>
+      </c>
+      <c r="E66" s="2">
+        <v>1.3720000000000001</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1.363</v>
+      </c>
+      <c r="G66" s="2">
+        <v>1.403</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B130" s="2"/>
+      <c r="C130" s="2"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B131" s="2"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B133" s="2"/>
+      <c r="C133" s="2"/>
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B134" s="2"/>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+    </row>
+    <row r="151" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+    </row>
+    <row r="152" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2"/>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+    </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+    </row>
+    <row r="156" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B156" s="2"/>
+      <c r="C156" s="2"/>
+      <c r="D156" s="2"/>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+    </row>
+    <row r="157" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B157" s="2"/>
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2"/>
+    </row>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B161" s="2"/>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B162" s="2"/>
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="2"/>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B163" s="2"/>
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="2"/>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2"/>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B166" s="2"/>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B167" s="2"/>
+      <c r="C167" s="2"/>
+      <c r="D167" s="2"/>
+      <c r="E167" s="2"/>
+      <c r="F167" s="2"/>
+      <c r="G167" s="2"/>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B168" s="2"/>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
+      <c r="G168" s="2"/>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B169" s="2"/>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="2"/>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B170" s="2"/>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="2"/>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B171" s="2"/>
+      <c r="C171" s="2"/>
+      <c r="D171" s="2"/>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
+      <c r="G171" s="2"/>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B172" s="2"/>
+      <c r="C172" s="2"/>
+      <c r="D172" s="2"/>
+      <c r="E172" s="2"/>
+      <c r="F172" s="2"/>
+      <c r="G172" s="2"/>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
+      <c r="D173" s="2"/>
+      <c r="E173" s="2"/>
+      <c r="F173" s="2"/>
+      <c r="G173" s="2"/>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B174" s="2"/>
+      <c r="C174" s="2"/>
+      <c r="D174" s="2"/>
+      <c r="E174" s="2"/>
+      <c r="F174" s="2"/>
+      <c r="G174" s="2"/>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B175" s="2"/>
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
+      <c r="E175" s="2"/>
+      <c r="F175" s="2"/>
+      <c r="G175" s="2"/>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
+      <c r="E176" s="2"/>
+      <c r="F176" s="2"/>
+      <c r="G176" s="2"/>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B177" s="2"/>
+      <c r="C177" s="2"/>
+      <c r="D177" s="2"/>
+      <c r="E177" s="2"/>
+      <c r="F177" s="2"/>
+      <c r="G177" s="2"/>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="2"/>
+      <c r="F178" s="2"/>
+      <c r="G178" s="2"/>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B179" s="2"/>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
+      <c r="E179" s="2"/>
+      <c r="F179" s="2"/>
+      <c r="G179" s="2"/>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="2"/>
+      <c r="F180" s="2"/>
+      <c r="G180" s="2"/>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B181" s="2"/>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="2"/>
+      <c r="F181" s="2"/>
+      <c r="G181" s="2"/>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B182" s="2"/>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
+      <c r="E182" s="2"/>
+      <c r="F182" s="2"/>
+      <c r="G182" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed example data to macth treatments
</commit_message>
<xml_diff>
--- a/sample_data/example_run1.xlsx
+++ b/sample_data/example_run1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic_Weizmann\WIS_pythonGabor\Coding\ODyssey\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDA9146-1540-4E1D-AA6A-F5D2C47E78D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287709C6-A1AD-46BB-9E6F-252A4FA04203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{83AB0913-2B68-40BB-A5C7-B40C6383A6EA}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,13 +488,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="E2" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F2" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F2" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
       <c r="G2" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -511,13 +511,13 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E3" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F3" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F3" s="1">
-        <v>6.0000000000000001E-3</v>
-      </c>
       <c r="G3" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -534,13 +534,13 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E4" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F4" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="G4" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -557,13 +557,13 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E5" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F5" s="1">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F5" s="1">
-        <v>8.9999999999999993E-3</v>
-      </c>
       <c r="G5" s="1">
-        <v>0.01</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -580,13 +580,13 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="E6" s="1">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F6" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F6" s="1">
-        <v>1.0999999999999999E-2</v>
-      </c>
       <c r="G6" s="1">
-        <v>1.2E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -603,10 +603,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="E7" s="1">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F7" s="1">
         <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1.4E-2</v>
       </c>
       <c r="G7" s="1">
         <v>1.6E-2</v>
@@ -626,13 +626,13 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E8" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="F8" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G8" s="1">
         <v>1.9E-2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -649,13 +649,13 @@
         <v>0.02</v>
       </c>
       <c r="E9" s="1">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G9" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -672,13 +672,13 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E10" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G10" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -695,13 +695,13 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>3.3000000000000002E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>4.5999999999999999E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="G11" s="1">
-        <v>0.05</v>
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -718,13 +718,13 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>4.2999999999999997E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>5.8999999999999997E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="G12" s="1">
-        <v>6.4000000000000001E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -741,13 +741,13 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>5.6000000000000001E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="G13" s="1">
-        <v>8.4000000000000005E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -764,13 +764,13 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>7.2999999999999995E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>0.10100000000000001</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="G14" s="1">
-        <v>0.11</v>
+        <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -787,13 +787,13 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="E15" s="1">
-        <v>9.8000000000000004E-2</v>
+        <v>0.113</v>
       </c>
       <c r="F15" s="1">
-        <v>0.13200000000000001</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="G15" s="1">
-        <v>0.14199999999999999</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -810,13 +810,13 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="E16" s="1">
-        <v>0.13</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="F16" s="1">
-        <v>0.17100000000000001</v>
+        <v>0.122</v>
       </c>
       <c r="G16" s="1">
-        <v>0.184</v>
+        <v>0.16600000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -833,13 +833,13 @@
         <v>0.17299999999999999</v>
       </c>
       <c r="E17" s="1">
-        <v>0.17</v>
+        <v>0.193</v>
       </c>
       <c r="F17" s="1">
-        <v>0.217</v>
+        <v>0.16</v>
       </c>
       <c r="G17" s="1">
-        <v>0.23100000000000001</v>
+        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -856,13 +856,13 @@
         <v>0.218</v>
       </c>
       <c r="E18" s="1">
-        <v>0.214</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="F18" s="1">
-        <v>0.25600000000000001</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="G18" s="1">
-        <v>0.27200000000000002</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -879,13 +879,13 @@
         <v>0.25900000000000001</v>
       </c>
       <c r="E19" s="1">
-        <v>0.25600000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F19" s="1">
-        <v>0.315</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="G19" s="1">
-        <v>0.33800000000000002</v>
+        <v>0.312</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -902,13 +902,13 @@
         <v>0.318</v>
       </c>
       <c r="E20" s="1">
-        <v>0.316</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="F20" s="1">
-        <v>0.372</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="G20" s="1">
-        <v>0.40100000000000002</v>
+        <v>0.376</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -925,13 +925,13 @@
         <v>0.371</v>
       </c>
       <c r="E21" s="1">
-        <v>0.373</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="F21" s="1">
-        <v>0.41699999999999998</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="G21" s="1">
-        <v>0.45</v>
+        <v>0.43099999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -948,13 +948,13 @@
         <v>0.41299999999999998</v>
       </c>
       <c r="E22" s="1">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F22" s="1">
         <v>0.41799999999999998</v>
       </c>
-      <c r="F22" s="1">
-        <v>0.46600000000000003</v>
-      </c>
       <c r="G22" s="1">
-        <v>0.5</v>
+        <v>0.48299999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -971,13 +971,13 @@
         <v>0.46400000000000002</v>
       </c>
       <c r="E23" s="1">
-        <v>0.46800000000000003</v>
+        <v>0.49</v>
       </c>
       <c r="F23" s="1">
-        <v>0.51300000000000001</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="G23" s="1">
-        <v>0.55300000000000005</v>
+        <v>0.54400000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -994,13 +994,13 @@
         <v>0.51500000000000001</v>
       </c>
       <c r="E24" s="1">
-        <v>0.51900000000000002</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="F24" s="1">
-        <v>0.57199999999999995</v>
+        <v>0.52400000000000002</v>
       </c>
       <c r="G24" s="1">
-        <v>0.61599999999999999</v>
+        <v>0.60199999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1017,13 +1017,13 @@
         <v>0.57399999999999995</v>
       </c>
       <c r="E25" s="1">
-        <v>0.57799999999999996</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="F25" s="1">
-        <v>0.624</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="G25" s="1">
-        <v>0.66900000000000004</v>
+        <v>0.65700000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1040,13 +1040,13 @@
         <v>0.63</v>
       </c>
       <c r="E26" s="1">
-        <v>0.63200000000000001</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="F26" s="1">
-        <v>0.67</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="G26" s="1">
-        <v>0.71799999999999997</v>
+        <v>0.71199999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1063,13 +1063,13 @@
         <v>0.68200000000000005</v>
       </c>
       <c r="E27" s="1">
-        <v>0.68</v>
+        <v>0.69</v>
       </c>
       <c r="F27" s="1">
-        <v>0.72599999999999998</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="G27" s="1">
-        <v>0.77700000000000002</v>
+        <v>0.77800000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1086,13 +1086,13 @@
         <v>0.749</v>
       </c>
       <c r="E28" s="1">
-        <v>0.74099999999999999</v>
+        <v>0.73</v>
       </c>
       <c r="F28" s="1">
-        <v>0.78400000000000003</v>
+        <v>0.753</v>
       </c>
       <c r="G28" s="1">
-        <v>0.82599999999999996</v>
+        <v>0.81599999999999995</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1109,13 +1109,13 @@
         <v>0.79</v>
       </c>
       <c r="E29" s="1">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="F29" s="1">
         <v>0.78900000000000003</v>
       </c>
-      <c r="F29" s="1">
-        <v>0.81200000000000006</v>
-      </c>
       <c r="G29" s="1">
-        <v>0.85</v>
+        <v>0.84099999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1132,13 +1132,13 @@
         <v>0.81599999999999995</v>
       </c>
       <c r="E30" s="1">
-        <v>0.82</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="F30" s="1">
-        <v>0.84199999999999997</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="G30" s="1">
-        <v>0.876</v>
+        <v>0.86599999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1155,13 +1155,13 @@
         <v>0.84399999999999997</v>
       </c>
       <c r="E31" s="1">
-        <v>0.85199999999999998</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="F31" s="1">
-        <v>0.871</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="G31" s="1">
-        <v>0.90200000000000002</v>
+        <v>0.89100000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1178,13 +1178,13 @@
         <v>0.86899999999999999</v>
       </c>
       <c r="E32" s="1">
-        <v>0.88700000000000001</v>
+        <v>0.78800000000000003</v>
       </c>
       <c r="F32" s="1">
-        <v>0.89300000000000002</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G32" s="1">
-        <v>0.92600000000000005</v>
+        <v>0.91600000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1201,13 +1201,13 @@
         <v>0.89900000000000002</v>
       </c>
       <c r="E33" s="1">
-        <v>0.91600000000000004</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="F33" s="1">
-        <v>0.91500000000000004</v>
+        <v>0.88</v>
       </c>
       <c r="G33" s="1">
-        <v>0.94899999999999995</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1224,13 +1224,13 @@
         <v>0.92700000000000005</v>
       </c>
       <c r="E34" s="1">
-        <v>0.94099999999999995</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="F34" s="1">
-        <v>0.93700000000000006</v>
+        <v>0.90300000000000002</v>
       </c>
       <c r="G34" s="1">
-        <v>0.97099999999999997</v>
+        <v>0.96399999999999997</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1247,13 +1247,13 @@
         <v>0.95399999999999996</v>
       </c>
       <c r="E35" s="1">
-        <v>0.95699999999999996</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="F35" s="1">
-        <v>0.95899999999999996</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="G35" s="1">
-        <v>0.99</v>
+        <v>0.99199999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1270,13 +1270,13 @@
         <v>0.98</v>
       </c>
       <c r="E36" s="1">
-        <v>0.97399999999999998</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="F36" s="1">
-        <v>0.98</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="G36" s="1">
-        <v>1.016</v>
+        <v>1.0149999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1293,13 +1293,13 @@
         <v>1.012</v>
       </c>
       <c r="E37" s="1">
-        <v>0.997</v>
+        <v>0.86799999999999999</v>
       </c>
       <c r="F37" s="1">
-        <v>1.0049999999999999</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="G37" s="1">
-        <v>1.038</v>
+        <v>1.0349999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1316,13 +1316,13 @@
         <v>1.032</v>
       </c>
       <c r="E38" s="1">
-        <v>1.016</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="F38" s="1">
-        <v>1.0369999999999999</v>
+        <v>0.996</v>
       </c>
       <c r="G38" s="1">
-        <v>1.0569999999999999</v>
+        <v>1.0529999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1339,13 +1339,13 @@
         <v>1.0549999999999999</v>
       </c>
       <c r="E39" s="1">
-        <v>1.0509999999999999</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="F39" s="1">
-        <v>1.0549999999999999</v>
+        <v>1.016</v>
       </c>
       <c r="G39" s="1">
-        <v>1.0740000000000001</v>
+        <v>1.071</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1362,13 +1362,13 @@
         <v>1.075</v>
       </c>
       <c r="E40" s="1">
-        <v>1.0680000000000001</v>
+        <v>0.91</v>
       </c>
       <c r="F40" s="1">
-        <v>1.069</v>
+        <v>1.0349999999999999</v>
       </c>
       <c r="G40" s="1">
-        <v>1.093</v>
+        <v>1.089</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1385,13 +1385,13 @@
         <v>1.095</v>
       </c>
       <c r="E41" s="1">
-        <v>1.0880000000000001</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="F41" s="1">
-        <v>1.0900000000000001</v>
+        <v>1.052</v>
       </c>
       <c r="G41" s="1">
-        <v>1.109</v>
+        <v>1.1080000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1408,13 +1408,13 @@
         <v>1.1120000000000001</v>
       </c>
       <c r="E42" s="1">
-        <v>1.109</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="F42" s="1">
-        <v>1.1060000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="G42" s="1">
-        <v>1.1259999999999999</v>
+        <v>1.123</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1431,13 +1431,13 @@
         <v>1.131</v>
       </c>
       <c r="E43" s="1">
-        <v>1.1279999999999999</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="F43" s="1">
-        <v>1.119</v>
+        <v>1.0880000000000001</v>
       </c>
       <c r="G43" s="1">
-        <v>1.1419999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1454,13 +1454,13 @@
         <v>1.149</v>
       </c>
       <c r="E44" s="1">
-        <v>1.1419999999999999</v>
+        <v>0.96699999999999997</v>
       </c>
       <c r="F44" s="1">
-        <v>1.135</v>
+        <v>1.1040000000000001</v>
       </c>
       <c r="G44" s="1">
-        <v>1.1579999999999999</v>
+        <v>1.155</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1477,13 +1477,13 @@
         <v>1.1639999999999999</v>
       </c>
       <c r="E45" s="1">
-        <v>1.1579999999999999</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="F45" s="1">
-        <v>1.149</v>
+        <v>1.121</v>
       </c>
       <c r="G45" s="1">
-        <v>1.1739999999999999</v>
+        <v>1.171</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1500,13 +1500,13 @@
         <v>1.1779999999999999</v>
       </c>
       <c r="E46" s="1">
-        <v>1.173</v>
+        <v>0.999</v>
       </c>
       <c r="F46" s="1">
-        <v>1.163</v>
+        <v>1.1359999999999999</v>
       </c>
       <c r="G46" s="1">
-        <v>1.19</v>
+        <v>1.1879999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1523,13 +1523,13 @@
         <v>1.1910000000000001</v>
       </c>
       <c r="E47" s="1">
-        <v>1.1870000000000001</v>
+        <v>1.018</v>
       </c>
       <c r="F47" s="1">
-        <v>1.177</v>
+        <v>1.151</v>
       </c>
       <c r="G47" s="1">
-        <v>1.204</v>
+        <v>1.2030000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1546,13 +1546,13 @@
         <v>1.2050000000000001</v>
       </c>
       <c r="E48" s="1">
-        <v>1.2010000000000001</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="F48" s="1">
-        <v>1.19</v>
+        <v>1.1659999999999999</v>
       </c>
       <c r="G48" s="1">
-        <v>1.2190000000000001</v>
+        <v>1.2210000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -1569,10 +1569,10 @@
         <v>1.2190000000000001</v>
       </c>
       <c r="E49" s="1">
-        <v>1.2150000000000001</v>
+        <v>1.0449999999999999</v>
       </c>
       <c r="F49" s="1">
-        <v>1.202</v>
+        <v>1.179</v>
       </c>
       <c r="G49" s="1">
         <v>1.234</v>
@@ -1592,13 +1592,13 @@
         <v>1.2310000000000001</v>
       </c>
       <c r="E50" s="1">
-        <v>1.2290000000000001</v>
+        <v>1.0620000000000001</v>
       </c>
       <c r="F50" s="1">
-        <v>1.212</v>
+        <v>1.194</v>
       </c>
       <c r="G50" s="1">
-        <v>1.2509999999999999</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -1615,13 +1615,13 @@
         <v>1.242</v>
       </c>
       <c r="E51" s="1">
-        <v>1.242</v>
+        <v>1.081</v>
       </c>
       <c r="F51" s="1">
-        <v>1.2230000000000001</v>
+        <v>1.2070000000000001</v>
       </c>
       <c r="G51" s="1">
-        <v>1.2609999999999999</v>
+        <v>1.264</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -1638,13 +1638,13 @@
         <v>1.254</v>
       </c>
       <c r="E52" s="1">
-        <v>1.254</v>
+        <v>1.091</v>
       </c>
       <c r="F52" s="1">
-        <v>1.234</v>
+        <v>1.22</v>
       </c>
       <c r="G52" s="1">
-        <v>1.272</v>
+        <v>1.2769999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -1661,13 +1661,13 @@
         <v>1.2649999999999999</v>
       </c>
       <c r="E53" s="1">
-        <v>1.2649999999999999</v>
+        <v>1.1060000000000001</v>
       </c>
       <c r="F53" s="1">
-        <v>1.2450000000000001</v>
+        <v>1.236</v>
       </c>
       <c r="G53" s="1">
-        <v>1.2889999999999999</v>
+        <v>1.2909999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -1684,13 +1684,13 @@
         <v>1.2749999999999999</v>
       </c>
       <c r="E54" s="1">
-        <v>1.2749999999999999</v>
+        <v>1.1180000000000001</v>
       </c>
       <c r="F54" s="1">
-        <v>1.254</v>
+        <v>1.248</v>
       </c>
       <c r="G54" s="1">
-        <v>1.294</v>
+        <v>1.304</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -1707,13 +1707,13 @@
         <v>1.2849999999999999</v>
       </c>
       <c r="E55" s="1">
-        <v>1.284</v>
+        <v>1.131</v>
       </c>
       <c r="F55" s="1">
-        <v>1.264</v>
+        <v>1.262</v>
       </c>
       <c r="G55" s="1">
-        <v>1.304</v>
+        <v>1.3140000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -1730,13 +1730,13 @@
         <v>1.2949999999999999</v>
       </c>
       <c r="E56" s="1">
-        <v>1.2929999999999999</v>
+        <v>1.1419999999999999</v>
       </c>
       <c r="F56" s="1">
-        <v>1.274</v>
+        <v>1.2729999999999999</v>
       </c>
       <c r="G56" s="1">
-        <v>1.3149999999999999</v>
+        <v>1.3260000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -1753,13 +1753,13 @@
         <v>1.3029999999999999</v>
       </c>
       <c r="E57" s="1">
-        <v>1.3009999999999999</v>
+        <v>1.153</v>
       </c>
       <c r="F57" s="1">
         <v>1.2829999999999999</v>
       </c>
       <c r="G57" s="1">
-        <v>1.3220000000000001</v>
+        <v>1.339</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -1776,13 +1776,13 @@
         <v>1.3120000000000001</v>
       </c>
       <c r="E58" s="1">
-        <v>1.3089999999999999</v>
+        <v>1.1659999999999999</v>
       </c>
       <c r="F58" s="1">
-        <v>1.292</v>
+        <v>1.294</v>
       </c>
       <c r="G58" s="1">
-        <v>1.331</v>
+        <v>1.347</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -1799,13 +1799,13 @@
         <v>1.321</v>
       </c>
       <c r="E59" s="1">
-        <v>1.3169999999999999</v>
+        <v>1.1779999999999999</v>
       </c>
       <c r="F59" s="1">
-        <v>1.3009999999999999</v>
+        <v>1.306</v>
       </c>
       <c r="G59" s="1">
-        <v>1.34</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -1822,13 +1822,13 @@
         <v>1.329</v>
       </c>
       <c r="E60" s="1">
-        <v>1.3260000000000001</v>
+        <v>1.1890000000000001</v>
       </c>
       <c r="F60" s="1">
-        <v>1.3089999999999999</v>
+        <v>1.3160000000000001</v>
       </c>
       <c r="G60" s="1">
-        <v>1.35</v>
+        <v>1.3680000000000001</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -1845,13 +1845,13 @@
         <v>1.337</v>
       </c>
       <c r="E61" s="1">
-        <v>1.333</v>
+        <v>1.2</v>
       </c>
       <c r="F61" s="1">
-        <v>1.3180000000000001</v>
+        <v>1.3260000000000001</v>
       </c>
       <c r="G61" s="1">
-        <v>1.359</v>
+        <v>1.379</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -1868,13 +1868,13 @@
         <v>1.345</v>
       </c>
       <c r="E62" s="1">
-        <v>1.341</v>
+        <v>1.2110000000000001</v>
       </c>
       <c r="F62" s="1">
-        <v>1.327</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="G62" s="1">
-        <v>1.369</v>
+        <v>1.389</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -1891,13 +1891,13 @@
         <v>1.353</v>
       </c>
       <c r="E63" s="1">
-        <v>1.3480000000000001</v>
+        <v>1.2230000000000001</v>
       </c>
       <c r="F63" s="1">
-        <v>1.337</v>
+        <v>1.347</v>
       </c>
       <c r="G63" s="1">
-        <v>1.3779999999999999</v>
+        <v>1.397</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -1914,13 +1914,13 @@
         <v>1.363</v>
       </c>
       <c r="E64" s="1">
+        <v>1.2330000000000001</v>
+      </c>
+      <c r="F64" s="1">
         <v>1.355</v>
       </c>
-      <c r="F64" s="1">
-        <v>1.345</v>
-      </c>
       <c r="G64" s="1">
-        <v>1.3879999999999999</v>
+        <v>1.4059999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -1937,13 +1937,13 @@
         <v>1.371</v>
       </c>
       <c r="E65" s="1">
-        <v>1.363</v>
+        <v>1.2430000000000001</v>
       </c>
       <c r="F65" s="1">
-        <v>1.3540000000000001</v>
+        <v>1.3640000000000001</v>
       </c>
       <c r="G65" s="1">
-        <v>1.3959999999999999</v>
+        <v>1.413</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -1960,13 +1960,13 @@
         <v>1.3779999999999999</v>
       </c>
       <c r="E66" s="1">
+        <v>1.252</v>
+      </c>
+      <c r="F66" s="1">
         <v>1.3720000000000001</v>
       </c>
-      <c r="F66" s="1">
-        <v>1.363</v>
-      </c>
       <c r="G66" s="1">
-        <v>1.403</v>
+        <v>1.423</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>